<commit_message>
feat: Implement email attachment collection logic and add a new configuration file.
</commit_message>
<xml_diff>
--- a/Data/Config.xlsx
+++ b/Data/Config.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\UiPath\Final Project\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{165E3F60-2214-43A8-8630-8638807E2A0F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E76961C-B599-4284-B611-7A9145713085}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -88,15 +88,15 @@
   </si>
   <si>
     <t>Orchestrator queue Name. The value must match with the queue name defined on Orchestrator.</t>
-    <phoneticPr fontId="5"/>
+    <phoneticPr fontId="6"/>
   </si>
   <si>
     <t>Logging field which allows grouping of log data of two or more subprocesses under the same business process name</t>
-    <phoneticPr fontId="5"/>
+    <phoneticPr fontId="6"/>
   </si>
   <si>
     <t>OrchestratorQueueName</t>
-    <phoneticPr fontId="5"/>
+    <phoneticPr fontId="6"/>
   </si>
   <si>
     <t>Must be 0 if working with Orchestrator queues. If &gt; 0, the robot will retry the same transaction which failed with a system exception. Must be an integer value.</t>
@@ -216,9 +216,6 @@
     <t>Scripts\generate_marksheet.py</t>
   </si>
   <si>
-    <t>Data\Output</t>
-  </si>
-  <si>
     <t>EmailTo</t>
   </si>
   <si>
@@ -247,17 +244,27 @@
   </si>
   <si>
     <t>port</t>
+  </si>
+  <si>
+    <t>F:\UiPath\Final Project\Data\Output</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="11"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
     <font>
       <sz val="11"/>
@@ -324,40 +331,43 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -675,8 +685,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:Z998"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.42578125" defaultRowHeight="15" customHeight="1"/>
@@ -785,8 +795,8 @@
       <c r="A8" s="4" t="s">
         <v>48</v>
       </c>
-      <c r="B8" s="7" t="s">
-        <v>63</v>
+      <c r="B8" s="13" t="s">
+        <v>73</v>
       </c>
       <c r="C8" s="4" t="s">
         <v>49</v>
@@ -849,46 +859,46 @@
     </row>
     <row r="14" spans="1:26" ht="14.25" customHeight="1">
       <c r="A14" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="B14" s="9" t="s">
         <v>64</v>
       </c>
-      <c r="B14" s="9" t="s">
-        <v>65</v>
-      </c>
       <c r="C14" s="8" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="15" spans="1:26" ht="14.25" customHeight="1">
       <c r="A15" s="8" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B15" s="9" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C15" s="8" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="16" spans="1:26" ht="14.25" customHeight="1">
       <c r="A16" s="10" t="s">
+        <v>66</v>
+      </c>
+      <c r="B16" s="8" t="s">
         <v>67</v>
       </c>
-      <c r="B16" s="8" t="s">
-        <v>68</v>
-      </c>
       <c r="C16" s="10" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="17" spans="1:3" ht="14.25" customHeight="1">
       <c r="A17" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B17" s="11">
         <v>587</v>
       </c>
       <c r="C17" s="10" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="18" spans="1:3" ht="14.25" customHeight="1">
@@ -1883,7 +1893,7 @@
     <row r="997" ht="14.25" customHeight="1"/>
     <row r="998" ht="14.25" customHeight="1"/>
   </sheetData>
-  <phoneticPr fontId="5"/>
+  <phoneticPr fontId="6"/>
   <hyperlinks>
     <hyperlink ref="B14" r:id="rId1" xr:uid="{B15561CD-3DA5-4FA5-96B8-DAAF4B347341}"/>
     <hyperlink ref="B15" r:id="rId2" xr:uid="{AF4446B2-F414-4CE3-B347-90811A70DFD0}"/>
@@ -3051,7 +3061,7 @@
     <row r="987" ht="14.25" customHeight="1"/>
     <row r="988" ht="14.25" customHeight="1"/>
   </sheetData>
-  <phoneticPr fontId="5"/>
+  <phoneticPr fontId="6"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4106,7 +4116,7 @@
     <row r="999" ht="14.25" customHeight="1"/>
     <row r="1000" ht="14.25" customHeight="1"/>
   </sheetData>
-  <phoneticPr fontId="5"/>
+  <phoneticPr fontId="6"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
</xml_diff>